<commit_message>
Prep Chargebacks for 20160620-20160722
as of July 19th @ 12:00 pm
</commit_message>
<xml_diff>
--- a/20160620/Daily_log_20160620.xlsx
+++ b/20160620/Daily_log_20160620.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="15210" yWindow="0" windowWidth="20700" windowHeight="9345"/>
+    <workbookView xWindow="17550" yWindow="0" windowWidth="20700" windowHeight="9345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -991,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E211"/>
+  <dimension ref="A1:E217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="A188" sqref="A188:XFD381"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A188" sqref="A188:A218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3648,7 +3648,7 @@
         <v>42569</v>
       </c>
       <c r="B187" s="2">
-        <v>0.70138888888888884</v>
+        <v>0.71666666666666667</v>
       </c>
       <c r="C187" t="s">
         <v>2</v>
@@ -3725,6 +3725,24 @@
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="1"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="1"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="1"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="1"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="1"/>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>